<commit_message>
Reconfigure isocline repo #1: 3-6-2025
</commit_message>
<xml_diff>
--- a/data/Growth_DataSheet_v5.xlsx
+++ b/data/Growth_DataSheet_v5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4f5e485ed766aa2/Pictures/Documents/Journal Publications/Manuscripts/LILA/Pomacea/Isocline_manuscript/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="567" documentId="13_ncr:1_{854A672A-3423-4591-8C78-C0ADEE945D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0127A7C-5E70-493D-8694-5B43389238D7}"/>
+  <xr:revisionPtr revIDLastSave="569" documentId="13_ncr:1_{854A672A-3423-4591-8C78-C0ADEE945D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7B8E930-2EBF-4BE8-9F18-9589F65D7EE8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="792" activeTab="3" xr2:uid="{8C70EDA9-54B7-4600-A91A-3B1148291D66}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" tabRatio="792" activeTab="5" xr2:uid="{8C70EDA9-54B7-4600-A91A-3B1148291D66}"/>
   </bookViews>
   <sheets>
     <sheet name="FieldData" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2248" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2246" uniqueCount="119">
   <si>
     <t>GROWTH EXPERIMENT DATA SHEET</t>
   </si>
@@ -684,14 +684,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -729,7 +725,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -835,7 +831,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -977,7 +973,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -16641,7 +16637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{335FBA75-6A00-4850-90A3-A1C89E6F7EE8}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E1048576"/>
     </sheetView>
   </sheetViews>
@@ -19058,8 +19054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA135D7-C820-4D81-BC0E-6B66FB414D0C}">
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19334,12 +19330,6 @@
         <f t="shared" si="2"/>
         <v>105.58450585894319</v>
       </c>
-      <c r="F4" t="s">
-        <v>101</v>
-      </c>
-      <c r="G4" t="s">
-        <v>79</v>
-      </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="s">

</xml_diff>